<commit_message>
Add o gráfico de medicamentos de Jacareí e formatei o de Aparecida
</commit_message>
<xml_diff>
--- a/Dados/Dados de Medicamentos/Gasto Medicamentos Finalizado - Aparecida.xlsx
+++ b/Dados/Dados de Medicamentos/Gasto Medicamentos Finalizado - Aparecida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120fd542a8b8b6a0/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5DFBFBA9-2A99-4D1F-8977-03CA2544ACB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC7C371-5B6D-4764-AB78-32CC444BF614}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{5DFBFBA9-2A99-4D1F-8977-03CA2544ACB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CED2D4E-42E4-497A-926B-1AF81587E621}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4044" yWindow="4044" windowWidth="17280" windowHeight="8880" xr2:uid="{17BB4940-856B-49AF-82F9-D7ED0FEB1D99}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{17BB4940-856B-49AF-82F9-D7ED0FEB1D99}"/>
   </bookViews>
   <sheets>
     <sheet name="TOTAL" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -132,23 +132,55 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
+              <a:rPr lang="pt-BR" sz="1600" b="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>Total</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> de gasto com medicamentos em Aparecida</a:t>
+              <a:rPr lang="pt-BR" sz="1600" b="0" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> de gastos com medicamentos</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="0" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> em Aparecida</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1600" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34829855643044622"/>
+          <c:y val="7.2964209010860148E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -169,9 +201,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -180,7 +212,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26488692038495187"/>
+          <c:y val="0.30559127538666131"/>
+          <c:w val="0.70455752405949257"/>
+          <c:h val="0.59484147435691626"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -384,36 +426,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -502,8 +514,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Gasto em reais</a:t>
+                  <a:t>Valor</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> gasto</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1172,8 +1189,8 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -1559,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C730FEA5-B52E-4F14-BE33-A3F7E8E5D75E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Remoção das pastas com os gráficos separadas por cidade
</commit_message>
<xml_diff>
--- a/Dados/Dados de Medicamentos/Gasto Medicamentos Finalizado - Aparecida.xlsx
+++ b/Dados/Dados de Medicamentos/Gasto Medicamentos Finalizado - Aparecida.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120fd542a8b8b6a0/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatec\Desktop\API\Dados\Dados de Medicamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{5DFBFBA9-2A99-4D1F-8977-03CA2544ACB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CED2D4E-42E4-497A-926B-1AF81587E621}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF938B3-79B7-423A-8C4D-040BB32A6E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{17BB4940-856B-49AF-82F9-D7ED0FEB1D99}"/>
+    <workbookView xWindow="11430" yWindow="0" windowWidth="11715" windowHeight="12330" xr2:uid="{17BB4940-856B-49AF-82F9-D7ED0FEB1D99}"/>
   </bookViews>
   <sheets>
     <sheet name="TOTAL" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,10 +26,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -177,8 +174,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.34829855643044622"/>
-          <c:y val="7.2964209010860148E-2"/>
+          <c:x val="0.23678081790324348"/>
+          <c:y val="4.8662948115689664E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -590,7 +587,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1224,57 +1221,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Despesas-Medicamentos-Aparecida"/>
-      <sheetName val="TOTAL"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="A2">
-            <v>2019</v>
-          </cell>
-          <cell r="B2">
-            <v>2198546.4500000002</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>2020</v>
-          </cell>
-          <cell r="B3">
-            <v>1325888.3700000001</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>2021</v>
-          </cell>
-          <cell r="B4">
-            <v>1288791.6200000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>2022</v>
-          </cell>
-          <cell r="B5">
-            <v>2337375.98</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1576,16 +1522,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C730FEA5-B52E-4F14-BE33-A3F7E8E5D75E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1601,7 +1547,7 @@
         <v>2198546.4500000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -1609,7 +1555,7 @@
         <v>1325888.3700000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -1617,7 +1563,7 @@
         <v>1288791.6200000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -1637,7 +1583,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>